<commit_message>
Test Case 11 deleted
</commit_message>
<xml_diff>
--- a/DataEngine.xlsx
+++ b/DataEngine.xlsx
@@ -1,28 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Working\Workspace_maven\SeleniumProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Working\selenium1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="2" windowHeight="5775" windowWidth="14790" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14790" windowHeight="5775"/>
   </bookViews>
   <sheets>
-    <sheet name="Executor" r:id="rId1" sheetId="1"/>
-    <sheet name="Component2" r:id="rId2" sheetId="4"/>
-    <sheet name="End to End" r:id="rId3" sheetId="2"/>
-    <sheet name="Setting" r:id="rId4" sheetId="3"/>
+    <sheet name="Executor" sheetId="1" r:id="rId1"/>
+    <sheet name="Component2" sheetId="4" r:id="rId2"/>
+    <sheet name="End to End" sheetId="2" r:id="rId3"/>
+    <sheet name="Setting" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="RunMode">Setting!$A$1:$A$4</definedName>
   </definedNames>
   <calcPr calcId="0"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="950" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="128">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -413,50 +413,13 @@
     <t>Test Case 10</t>
   </si>
   <si>
-    <t>TC011</t>
-  </si>
-  <si>
-    <t>Test Case 11</t>
-  </si>
-  <si>
-    <t>https://www.healthquotes.ca/</t>
-  </si>
-  <si>
-    <t>btn_quote</t>
-  </si>
-  <si>
-    <t>Click on quote</t>
-  </si>
-  <si>
-    <t>Click on instant quote</t>
-  </si>
-  <si>
-    <t>btn_instant</t>
-  </si>
-  <si>
-    <t>btn_get_quote</t>
-  </si>
-  <si>
-    <t>optional_text</t>
-  </si>
-  <si>
-    <t>Please select your province/territory.</t>
-  </si>
-  <si>
     <t>Skipped</t>
-  </si>
-  <si>
-    <t>Error</t>
-  </si>
-  <si>
-    <t>Fail</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -519,7 +482,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -566,45 +529,82 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="3" numFmtId="49" xfId="0"/>
-    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="4" numFmtId="49" xfId="0"/>
-    <xf applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="4" numFmtId="49" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="4" numFmtId="49" xfId="0"/>
-    <xf applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="5" numFmtId="49" xfId="1"/>
-    <xf applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="3" numFmtId="49" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="4" numFmtId="49" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="3" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="3" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="1" numFmtId="49" xfId="0"/>
-    <xf applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="1" numFmtId="49" xfId="0"/>
-    <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="2" numFmtId="49" xfId="1"/>
-    <xf applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="3" numFmtId="49" xfId="0">
+  <cellXfs count="20">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -621,10 +621,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -659,7 +659,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -711,7 +711,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -822,21 +822,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -853,7 +853,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -905,27 +905,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -965,7 +965,7 @@
         <v>42</v>
       </c>
       <c r="F2" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -985,7 +985,7 @@
         <v>42</v>
       </c>
       <c r="F3" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1005,7 +1005,7 @@
         <v>42</v>
       </c>
       <c r="F4" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1025,7 +1025,7 @@
         <v>42</v>
       </c>
       <c r="F5" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1045,7 +1045,7 @@
         <v>42</v>
       </c>
       <c r="F6" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1065,7 +1065,7 @@
         <v>42</v>
       </c>
       <c r="F7" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1085,7 +1085,7 @@
         <v>42</v>
       </c>
       <c r="F8" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1105,7 +1105,7 @@
         <v>42</v>
       </c>
       <c r="F9" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1125,7 +1125,7 @@
         <v>42</v>
       </c>
       <c r="F10" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1145,70 +1145,50 @@
         <v>42</v>
       </c>
       <c r="F11" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
         <v>127</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>128</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="E12" t="s">
-        <v>2</v>
-      </c>
-      <c r="F12" t="s">
-        <v>139</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="E1:E1048576" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1048576">
       <formula1>RunMode</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:U111"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:T100"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A92" workbookViewId="0">
-      <selection activeCell="J107" sqref="J107"/>
+    <sheetView showGridLines="0" topLeftCell="A57" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E115" sqref="E115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="7" width="11.0" collapsed="true"/>
-    <col min="2" max="2" style="7" width="8.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="7" width="23.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="7" width="16.28515625" collapsed="true"/>
-    <col min="5" max="8" customWidth="true" style="7" width="14.85546875" collapsed="true"/>
-    <col min="9" max="10" style="7" width="8.85546875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="7" width="9.5703125" collapsed="true"/>
-    <col min="12" max="16384" style="7" width="8.85546875" collapsed="true"/>
+    <col min="1" max="1" width="11" style="7" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="8.85546875" style="7" collapsed="1"/>
+    <col min="3" max="3" width="23.42578125" style="7" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.28515625" style="7" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="8" width="14.85546875" style="7" customWidth="1" collapsed="1"/>
+    <col min="9" max="10" width="8.85546875" style="7" collapsed="1"/>
+    <col min="11" max="11" width="9.5703125" style="7" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="16384" width="8.85546875" style="7" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
@@ -1250,20 +1230,20 @@
       <c r="J3" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="K3" s="22" t="s">
+      <c r="K3" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="L3" s="22"/>
-      <c r="M3" s="22"/>
-      <c r="N3" s="22"/>
-      <c r="O3" s="22"/>
-      <c r="P3" s="22" t="s">
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="18"/>
+      <c r="O3" s="19"/>
+      <c r="P3" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="Q3" s="22"/>
-      <c r="R3" s="22"/>
-      <c r="S3" s="22"/>
-      <c r="T3" s="22"/>
+      <c r="Q3" s="18"/>
+      <c r="R3" s="18"/>
+      <c r="S3" s="18"/>
+      <c r="T3" s="19"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -1628,20 +1608,20 @@
       <c r="J15" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="K15" s="22" t="s">
+      <c r="K15" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="L15" s="22"/>
-      <c r="M15" s="22"/>
-      <c r="N15" s="22"/>
-      <c r="O15" s="22"/>
-      <c r="P15" s="22" t="s">
+      <c r="L15" s="18"/>
+      <c r="M15" s="18"/>
+      <c r="N15" s="18"/>
+      <c r="O15" s="19"/>
+      <c r="P15" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="Q15" s="22"/>
-      <c r="R15" s="22"/>
-      <c r="S15" s="22"/>
-      <c r="T15" s="22"/>
+      <c r="Q15" s="18"/>
+      <c r="R15" s="18"/>
+      <c r="S15" s="18"/>
+      <c r="T15" s="19"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
@@ -1922,20 +1902,20 @@
       <c r="J24" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="K24" s="22" t="s">
+      <c r="K24" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="L24" s="22"/>
-      <c r="M24" s="22"/>
-      <c r="N24" s="22"/>
-      <c r="O24" s="22"/>
-      <c r="P24" s="22" t="s">
+      <c r="L24" s="18"/>
+      <c r="M24" s="18"/>
+      <c r="N24" s="18"/>
+      <c r="O24" s="19"/>
+      <c r="P24" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="Q24" s="22"/>
-      <c r="R24" s="22"/>
-      <c r="S24" s="22"/>
-      <c r="T24" s="22"/>
+      <c r="Q24" s="18"/>
+      <c r="R24" s="18"/>
+      <c r="S24" s="18"/>
+      <c r="T24" s="19"/>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
@@ -2249,18 +2229,18 @@
       <c r="J34" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="K34" s="22" t="s">
+      <c r="K34" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="L34" s="22"/>
-      <c r="M34" s="22"/>
-      <c r="N34" s="22"/>
-      <c r="O34" s="22"/>
-      <c r="P34" s="22"/>
-      <c r="Q34" s="22"/>
-      <c r="R34" s="22"/>
-      <c r="S34" s="22"/>
-      <c r="T34" s="22"/>
+      <c r="L34" s="18"/>
+      <c r="M34" s="18"/>
+      <c r="N34" s="18"/>
+      <c r="O34" s="19"/>
+      <c r="P34" s="17"/>
+      <c r="Q34" s="18"/>
+      <c r="R34" s="18"/>
+      <c r="S34" s="18"/>
+      <c r="T34" s="19"/>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
@@ -2584,13 +2564,13 @@
       <c r="J44" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="K44" s="22" t="s">
+      <c r="K44" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="L44" s="22"/>
-      <c r="M44" s="22"/>
-      <c r="N44" s="22"/>
-      <c r="O44" s="22"/>
+      <c r="L44" s="18"/>
+      <c r="M44" s="18"/>
+      <c r="N44" s="18"/>
+      <c r="O44" s="19"/>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
@@ -2624,11 +2604,11 @@
       <c r="M45" s="8"/>
       <c r="N45" s="8"/>
       <c r="O45" s="8"/>
-      <c r="P45" s="22"/>
-      <c r="Q45" s="22"/>
-      <c r="R45" s="22"/>
-      <c r="S45" s="22"/>
-      <c r="T45" s="22"/>
+      <c r="P45" s="17"/>
+      <c r="Q45" s="18"/>
+      <c r="R45" s="18"/>
+      <c r="S45" s="18"/>
+      <c r="T45" s="19"/>
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
@@ -2830,13 +2810,13 @@
       <c r="J52" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="K52" s="22" t="s">
+      <c r="K52" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="L52" s="22"/>
-      <c r="M52" s="22"/>
-      <c r="N52" s="22"/>
-      <c r="O52" s="22"/>
+      <c r="L52" s="18"/>
+      <c r="M52" s="18"/>
+      <c r="N52" s="18"/>
+      <c r="O52" s="19"/>
     </row>
     <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
@@ -2870,11 +2850,11 @@
       <c r="M53" s="8"/>
       <c r="N53" s="8"/>
       <c r="O53" s="8"/>
-      <c r="P53" s="22"/>
-      <c r="Q53" s="22"/>
-      <c r="R53" s="22"/>
-      <c r="S53" s="22"/>
-      <c r="T53" s="22"/>
+      <c r="P53" s="17"/>
+      <c r="Q53" s="18"/>
+      <c r="R53" s="18"/>
+      <c r="S53" s="18"/>
+      <c r="T53" s="19"/>
     </row>
     <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54" s="8" t="s">
@@ -3083,13 +3063,13 @@
       <c r="J60" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="K60" s="22" t="s">
+      <c r="K60" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="L60" s="22"/>
-      <c r="M60" s="22"/>
-      <c r="N60" s="22"/>
-      <c r="O60" s="22"/>
+      <c r="L60" s="18"/>
+      <c r="M60" s="18"/>
+      <c r="N60" s="18"/>
+      <c r="O60" s="19"/>
       <c r="P60" s="8"/>
       <c r="Q60" s="8"/>
       <c r="R60" s="8"/>
@@ -3349,13 +3329,13 @@
       <c r="J69" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="K69" s="22" t="s">
+      <c r="K69" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="L69" s="22"/>
-      <c r="M69" s="22"/>
-      <c r="N69" s="22"/>
-      <c r="O69" s="22"/>
+      <c r="L69" s="18"/>
+      <c r="M69" s="18"/>
+      <c r="N69" s="18"/>
+      <c r="O69" s="19"/>
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70" s="8" t="s">
@@ -3602,13 +3582,13 @@
       <c r="J78" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="K78" s="22" t="s">
+      <c r="K78" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="L78" s="22"/>
-      <c r="M78" s="22"/>
-      <c r="N78" s="22"/>
-      <c r="O78" s="22"/>
+      <c r="L78" s="18"/>
+      <c r="M78" s="18"/>
+      <c r="N78" s="18"/>
+      <c r="O78" s="19"/>
     </row>
     <row r="79" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A79" s="8" t="s">
@@ -3962,13 +3942,13 @@
       <c r="J90" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="K90" s="22" t="s">
+      <c r="K90" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="L90" s="22"/>
-      <c r="M90" s="22"/>
-      <c r="N90" s="22"/>
-      <c r="O90" s="22"/>
+      <c r="L90" s="18"/>
+      <c r="M90" s="18"/>
+      <c r="N90" s="18"/>
+      <c r="O90" s="19"/>
     </row>
     <row r="91" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A91" s="8" t="s">
@@ -4283,374 +4263,48 @@
         <v>34</v>
       </c>
     </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A101" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="B101" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A102" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B102" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C102" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D102" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E102" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="F102" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G102" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="H102" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="I102" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="J102" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="K102" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="L102" s="22"/>
-      <c r="M102" s="22"/>
-      <c r="N102" s="22"/>
-      <c r="O102" s="22"/>
-    </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A103" s="18" t="s">
-        <v>127</v>
-      </c>
-      <c r="B103" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C103" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D103" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="E103" s="8"/>
-      <c r="F103" s="8"/>
-      <c r="G103" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="H103" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="I103" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="J103" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="K103" s="10"/>
-      <c r="L103" s="8"/>
-      <c r="M103" s="8"/>
-      <c r="N103" s="8"/>
-      <c r="O103" s="8"/>
-    </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A104" s="18" t="s">
-        <v>127</v>
-      </c>
-      <c r="B104" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C104" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D104" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E104" s="8"/>
-      <c r="F104" s="8"/>
-      <c r="G104" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="H104" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="I104" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="J104" t="s">
-        <v>123</v>
-      </c>
-      <c r="K104" s="20" t="s">
-        <v>129</v>
-      </c>
-      <c r="L104" s="8"/>
-      <c r="M104" s="8"/>
-      <c r="N104" s="8"/>
-      <c r="O104" s="8"/>
-    </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A105" s="18" t="s">
-        <v>127</v>
-      </c>
-      <c r="B105" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C105" s="18" t="s">
-        <v>131</v>
-      </c>
-      <c r="D105" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="E105" s="18" t="s">
-        <v>117</v>
-      </c>
-      <c r="F105" s="21" t="s">
-        <v>130</v>
-      </c>
-      <c r="G105" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="H105" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="I105" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="J105" s="8"/>
-      <c r="K105" s="11"/>
-      <c r="L105" s="8"/>
-      <c r="M105" s="8"/>
-      <c r="N105" s="8"/>
-      <c r="O105" s="8"/>
-    </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A106" s="18" t="s">
-        <v>127</v>
-      </c>
-      <c r="B106" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C106" s="18" t="s">
-        <v>132</v>
-      </c>
-      <c r="D106" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="E106" s="18" t="s">
-        <v>117</v>
-      </c>
-      <c r="F106" s="21" t="s">
-        <v>133</v>
-      </c>
-      <c r="G106" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="H106" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="I106" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="J106" s="8"/>
-      <c r="K106" s="8"/>
-      <c r="L106" s="8"/>
-      <c r="M106" s="8"/>
-      <c r="N106" s="8"/>
-      <c r="O106" s="8"/>
-    </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A107" s="18" t="s">
-        <v>127</v>
-      </c>
-      <c r="B107" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C107" s="18" t="s">
-        <v>114</v>
-      </c>
-      <c r="D107" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="E107" s="18" t="s">
-        <v>117</v>
-      </c>
-      <c r="F107" s="21" t="s">
-        <v>134</v>
-      </c>
-      <c r="G107" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="H107" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="I107" s="23" t="s">
-        <v>124</v>
-      </c>
-      <c r="J107" t="s">
-        <v>123</v>
-      </c>
-      <c r="K107" s="8"/>
-      <c r="L107" s="8"/>
-      <c r="M107" s="8"/>
-      <c r="N107" s="8"/>
-      <c r="O107" s="8"/>
-    </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A108" s="18" t="s">
-        <v>127</v>
-      </c>
-      <c r="B108" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="C108" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="D108" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="E108" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="F108" s="18" t="s">
-        <v>135</v>
-      </c>
-      <c r="G108" s="13" t="s">
-        <v>136</v>
-      </c>
-      <c r="H108" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="I108" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="J108" t="s">
-        <v>123</v>
-      </c>
-      <c r="K108" s="18"/>
-      <c r="L108" s="8"/>
-      <c r="M108" s="8"/>
-      <c r="N108" s="8"/>
-      <c r="O108" s="8"/>
-    </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A109" s="18" t="s">
-        <v>127</v>
-      </c>
-      <c r="B109" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C109" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D109" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="E109" s="8"/>
-      <c r="F109" s="8"/>
-      <c r="G109" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="H109" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="I109" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="J109" s="8"/>
-      <c r="K109" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="L109" s="8"/>
-      <c r="M109" s="8"/>
-      <c r="N109" s="8"/>
-      <c r="O109" s="8"/>
-    </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A110" s="18" t="s">
-        <v>127</v>
-      </c>
-      <c r="B110" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C110" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D110" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="E110" s="8"/>
-      <c r="F110" s="8"/>
-      <c r="G110" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="H110" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="I110" s="9" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A111" s="19" t="s">
-        <v>128</v>
-      </c>
-      <c r="B111" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="17">
-    <mergeCell ref="K102:O102"/>
-    <mergeCell ref="K90:O90"/>
-    <mergeCell ref="K78:O78"/>
-    <mergeCell ref="K69:O69"/>
-    <mergeCell ref="K60:O60"/>
+  <mergeCells count="16">
+    <mergeCell ref="P53:T53"/>
+    <mergeCell ref="K34:O34"/>
+    <mergeCell ref="P34:T34"/>
+    <mergeCell ref="P45:T45"/>
+    <mergeCell ref="K44:O44"/>
+    <mergeCell ref="K52:O52"/>
     <mergeCell ref="K3:O3"/>
     <mergeCell ref="P3:T3"/>
     <mergeCell ref="K15:O15"/>
     <mergeCell ref="P15:T15"/>
     <mergeCell ref="K24:O24"/>
     <mergeCell ref="P24:T24"/>
-    <mergeCell ref="P53:T53"/>
-    <mergeCell ref="K34:O34"/>
-    <mergeCell ref="P34:T34"/>
-    <mergeCell ref="P45:T45"/>
-    <mergeCell ref="K44:O44"/>
-    <mergeCell ref="K52:O52"/>
+    <mergeCell ref="K90:O90"/>
+    <mergeCell ref="K78:O78"/>
+    <mergeCell ref="K69:O69"/>
+    <mergeCell ref="K60:O60"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="K8"/>
-    <hyperlink r:id="rId2" ref="K5"/>
-    <hyperlink location="/login/" r:id="rId3" ref="K17"/>
-    <hyperlink location="/login/" r:id="rId4" ref="K26"/>
-    <hyperlink location="/login/" r:id="rId5" ref="K36"/>
-    <hyperlink r:id="rId6" ref="K37"/>
-    <hyperlink location="/login/" r:id="rId7" ref="K46"/>
-    <hyperlink location="/login/" r:id="rId8" ref="K54"/>
-    <hyperlink location="/login/" r:id="rId9" ref="K62"/>
-    <hyperlink location="/login/" r:id="rId10" ref="K71"/>
-    <hyperlink r:id="rId11" ref="K80"/>
-    <hyperlink r:id="rId12" ref="K92"/>
-    <hyperlink r:id="rId13" ref="K104"/>
+    <hyperlink ref="K104" r:id="rId1" display="https://www.healthquotes.ca/"/>
+    <hyperlink ref="K92" r:id="rId2"/>
+    <hyperlink ref="K80" r:id="rId3"/>
+    <hyperlink ref="K71" r:id="rId4" location="/login/"/>
+    <hyperlink ref="K62" r:id="rId5" location="/login/"/>
+    <hyperlink ref="K54" r:id="rId6" location="/login/"/>
+    <hyperlink ref="K46" r:id="rId7" location="/login/"/>
+    <hyperlink ref="K37" r:id="rId8"/>
+    <hyperlink ref="K36" r:id="rId9" location="/login/"/>
+    <hyperlink ref="K26" r:id="rId10" location="/login/"/>
+    <hyperlink ref="K17" r:id="rId11" location="/login/"/>
+    <hyperlink ref="K5" r:id="rId12"/>
+    <hyperlink ref="K8" r:id="rId13"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId14"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
@@ -4658,9 +4312,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -4711,6 +4365,6 @@
   <sortState ref="A2:A4">
     <sortCondition ref="A2:A4"/>
   </sortState>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Test Case run mode change
</commit_message>
<xml_diff>
--- a/DataEngine.xlsx
+++ b/DataEngine.xlsx
@@ -916,7 +916,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -942,7 +942,7 @@
         <v>28</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>1</v>
@@ -1002,7 +1002,7 @@
         <v>50</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>42</v>
+        <v>2</v>
       </c>
       <c r="F4" t="s">
         <v>127</v>
@@ -1062,7 +1062,7 @@
         <v>50</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>42</v>
+        <v>2</v>
       </c>
       <c r="F7" t="s">
         <v>127</v>
@@ -1142,7 +1142,7 @@
         <v>50</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>42</v>
+        <v>2</v>
       </c>
       <c r="F11" t="s">
         <v>127</v>
@@ -4265,22 +4265,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="K90:O90"/>
+    <mergeCell ref="K78:O78"/>
+    <mergeCell ref="K69:O69"/>
+    <mergeCell ref="K60:O60"/>
+    <mergeCell ref="K3:O3"/>
+    <mergeCell ref="P3:T3"/>
+    <mergeCell ref="K15:O15"/>
+    <mergeCell ref="P15:T15"/>
+    <mergeCell ref="K24:O24"/>
+    <mergeCell ref="P24:T24"/>
     <mergeCell ref="P53:T53"/>
     <mergeCell ref="K34:O34"/>
     <mergeCell ref="P34:T34"/>
     <mergeCell ref="P45:T45"/>
     <mergeCell ref="K44:O44"/>
     <mergeCell ref="K52:O52"/>
-    <mergeCell ref="K3:O3"/>
-    <mergeCell ref="P3:T3"/>
-    <mergeCell ref="K15:O15"/>
-    <mergeCell ref="P15:T15"/>
-    <mergeCell ref="K24:O24"/>
-    <mergeCell ref="P24:T24"/>
-    <mergeCell ref="K90:O90"/>
-    <mergeCell ref="K78:O78"/>
-    <mergeCell ref="K69:O69"/>
-    <mergeCell ref="K60:O60"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="K104" r:id="rId1" display="https://www.healthquotes.ca/"/>

</xml_diff>